<commit_message>
add 2,3 embedding file for template search
</commit_message>
<xml_diff>
--- a/output/frat/conceptnet-local_embedding_search/depth_1/embeddings/frat_2,3_conceptnet_search_top10_merged-True_embeddings.xlsx
+++ b/output/frat/conceptnet-local_embedding_search/depth_1/embeddings/frat_2,3_conceptnet_search_top10_merged-True_embeddings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\conceptnet-local_embedding_search\depth_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\conceptnet-local_embedding_search\depth_1\embeddings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046AFA9-E127-4147-9129-9EE330C71FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC1062E-FB08-4927-BDBB-EABB16F0821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1128,7 +1128,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="37.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="33.90625" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" customWidth="1"/>
+    <col min="6" max="6" width="62.453125" customWidth="1"/>
+    <col min="7" max="7" width="52.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>